<commit_message>
inserted reuse businesses 1-13
</commit_message>
<xml_diff>
--- a/.wmi/other/ReUse-repair App documents.xlsx
+++ b/.wmi/other/ReUse-repair App documents.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="307" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="661" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Reuse Directory " sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="606">
   <si>
     <r>
       <t xml:space="preserve">CORVALLIS-AREA </t>
@@ -205,43 +205,43 @@
     </r>
   </si>
   <si>
-    <t>Albany-Corvallis ReUseIt (free items:  groups.yahoo.com)</t>
-  </si>
-  <si>
-    <t>Arc Thrift Stores (NW Beca-Corvallis, Main St-Philomath)</t>
-  </si>
-  <si>
-    <t>Beekman Place Antique Mall (601 SW Western Blvd)</t>
-  </si>
-  <si>
-    <t>Benton County Extension / 4-H  Activities (1849 NW 9th)</t>
-  </si>
-  <si>
-    <t>Benton County Master Gardeners (1849 NW 9th St)</t>
-  </si>
-  <si>
-    <t>Book Bin and Browser's Bookstore (both on 4th St)</t>
-  </si>
-  <si>
-    <t>Boys &amp; Girls Club / STARS (after school programs)</t>
-  </si>
-  <si>
-    <t>Buckingham Palace --Fri-Sun only (600 SW 3rd St)</t>
-  </si>
-  <si>
-    <t>CARDV (Center Against Rape/Domestic Violence)</t>
-  </si>
-  <si>
-    <t>Career Closet for Women (drop-off at 942 NW 9th, Ste.A)</t>
-  </si>
-  <si>
-    <t>Cat's Meow Humane Society Thrift Shop (411 SW 3rd St)</t>
-  </si>
-  <si>
-    <t>Children's Farm Home (Hway 20 btw Corvallis &amp; Albany)</t>
-  </si>
-  <si>
-    <t>Chintimini Wildlife Rehabilitation Ctr (311 Lewisburg Rd)</t>
+    <t>Albany-Corvallis ReUseIt (free items:  groups.yahoo.com1</t>
+  </si>
+  <si>
+    <t>Arc Thrift Stores (NW Beca-Corvallis, Main St-Philomath)2,3</t>
+  </si>
+  <si>
+    <t>Beekman Place Antique Mall (601 SW Western Blvd) 4</t>
+  </si>
+  <si>
+    <t>Benton County Extension / 4-H  Activities (1849 NW 9th)5</t>
+  </si>
+  <si>
+    <t>Benton County Master Gardeners (1849 NW 9th St)6</t>
+  </si>
+  <si>
+    <t>Book Bin and Browser's Bookstore (both on 4th St)7</t>
+  </si>
+  <si>
+    <t>Boys &amp; Girls Club / STARS (after school programs)9</t>
+  </si>
+  <si>
+    <t>Buckingham Palace --Fri-Sun only (600 SW 3rd St)10</t>
+  </si>
+  <si>
+    <t>CARDV (Center Against Rape/Domestic Violence)12</t>
+  </si>
+  <si>
+    <t>Career Closet for Women (drop-off at 942 NW 9th, Ste.A)13</t>
+  </si>
+  <si>
+    <t>Cat's Meow Humane Society Thrift Shop (411 SW 3rd St)14</t>
+  </si>
+  <si>
+    <t>Children's Farm Home (Hway 20 btw Corvallis &amp; Albany)15</t>
+  </si>
+  <si>
+    <t>Chintimini Wildlife Rehabilitation Ctr (311 Lewisburg Rd)16</t>
   </si>
   <si>
     <r>
@@ -255,44 +255,44 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">865 NW Reiman)</t>
+      <t xml:space="preserve">865 NW Reiman)17</t>
     </r>
   </si>
   <si>
-    <t>Corvallis Environmental Center (214 SW Monroe Ave)</t>
-  </si>
-  <si>
-    <t>Corvallis Bicycle Collective (33900 SE Roche Ln/Hwy 34)</t>
-  </si>
-  <si>
-    <t>CorvallisFurniture.com (720 NE Granger Ave, Bldg J)</t>
-  </si>
-  <si>
-    <t>Corvallis-Uzhhorod Sister Cities/The TOUCH Project</t>
-  </si>
-  <si>
-    <t>Cosmic Chameleon (138 SW 2nd St)</t>
-  </si>
-  <si>
-    <t>Craigslist (corvallis.craigslist.org) and Freecycle.org</t>
-  </si>
-  <si>
-    <t>First Alternative Co-op Recycling Center (1007 SE 3rd St)</t>
-  </si>
-  <si>
-    <t>First Alternative Co-op Stores (on NW Grant &amp; SE 3rd)</t>
-  </si>
-  <si>
-    <t>Furniture Exchange (210 NE 2nd St.)</t>
-  </si>
-  <si>
-    <t>Furniture Share (formerly Benton FS) (155 SE Lilly Ave)</t>
-  </si>
-  <si>
-    <t>Garland Nursery, Home Grown Gardens, etc.</t>
-  </si>
-  <si>
-    <t>Goodwill Industries (1325 NW 9th St)</t>
+    <t>Corvallis Environmental Center (214 SW Monroe Ave)18</t>
+  </si>
+  <si>
+    <t>Corvallis Bicycle Collective (33900 SE Roche Ln/Hwy 34)19</t>
+  </si>
+  <si>
+    <t>CorvallisFurniture.com (720 NE Granger Ave, Bldg J)20</t>
+  </si>
+  <si>
+    <t>Corvallis-Uzhhorod Sister Cities/The TOUCH Project21</t>
+  </si>
+  <si>
+    <t>Cosmic Chameleon (138 SW 2nd St)22</t>
+  </si>
+  <si>
+    <t>Craigslist (corvallis.craigslist.org) and Freecycle.org23</t>
+  </si>
+  <si>
+    <t>First Alternative Co-op Recycling Center (1007 SE 3rd St)24</t>
+  </si>
+  <si>
+    <t>First Alternative Co-op Stores (on NW Grant &amp; SE 3rd)24,25</t>
+  </si>
+  <si>
+    <t>Furniture Exchange (210 NE 2nd St.)27</t>
+  </si>
+  <si>
+    <t>Furniture Share (formerly Benton FS) (155 SE Lilly Ave)28</t>
+  </si>
+  <si>
+    <t>Garland Nursery, Home Grown Gardens, etc.29</t>
+  </si>
+  <si>
+    <t>Goodwill Industries (1325 NW 9th St)30</t>
   </si>
   <si>
     <r>
@@ -306,20 +306,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">4840 SW Philomath Blvd.)</t>
+      <t xml:space="preserve">4840 SW Philomath Blvd.)32</t>
     </r>
   </si>
   <si>
-    <t>Happy Trails Records, Tapes &amp; CDs (100 SW 3rd St)</t>
-  </si>
-  <si>
-    <t>Heartland Humane Society (398 SW Twin Oaks Cir)</t>
-  </si>
-  <si>
-    <t>Home Life Inc. (for develop. disabled, 2068 NW Fillmore)</t>
-  </si>
-  <si>
-    <t>Jackson Street Youth Shelter (555 NW Jackson St)</t>
+    <t>Happy Trails Records, Tapes &amp; CDs (100 SW 3rd St)33</t>
+  </si>
+  <si>
+    <t>Heartland Humane Society (398 SW Twin Oaks Cir)34</t>
+  </si>
+  <si>
+    <t>Home Life Inc. (for develop. disabled, 2068 NW Fillmore)35</t>
+  </si>
+  <si>
+    <t>Jackson Street Youth Shelter (555 NW Jackson St)36</t>
   </si>
   <si>
     <r>
@@ -333,23 +333,23 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">545 SW 2nd)</t>
+      <t xml:space="preserve">545 SW 2nd)37</t>
     </r>
   </si>
   <si>
-    <t>Lions Club (box inside Elks Lodge, 1400 NW 9th St)</t>
-  </si>
-  <si>
-    <t>Love INC (for low income citizens, 2330 NW Profess. Dr)</t>
-  </si>
-  <si>
-    <t>Mario Pastega House (Good Sam patient family housing)</t>
-  </si>
-  <si>
-    <t>Mary's River Gleaners (for low income citizens)</t>
-  </si>
-  <si>
-    <t>Midway Farms (Hway 20 btw Corvallis &amp; Albany)</t>
+    <t>Lions Club (box inside Elks Lodge, 1400 NW 9th St)38</t>
+  </si>
+  <si>
+    <t>Love INC (for low income citizens, 2330 NW Profess. Dr)39</t>
+  </si>
+  <si>
+    <t>Mario Pastega House (Good Sam patient family housing)40</t>
+  </si>
+  <si>
+    <t>Mary's River Gleaners (for low income citizens)41</t>
+  </si>
+  <si>
+    <t>Midway Farms (Hway 20 btw Corvallis &amp; Albany)42</t>
   </si>
   <si>
     <r>
@@ -371,47 +371,47 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)</t>
+      <t xml:space="preserve">)43</t>
     </r>
   </si>
   <si>
-    <t>Osborn Aquatic Center (1940 NW Highland Dr)</t>
-  </si>
-  <si>
-    <t>OSU Emergency Food Pantry (2150 SW Jefferson Way)</t>
-  </si>
-  <si>
-    <t>OSU Folk Club Thrift Shop (144 NW 2nd St)</t>
-  </si>
-  <si>
-    <t>OSU Organic Growers Club (Crop &amp; Soil Science Dep't)</t>
-  </si>
-  <si>
-    <t>Pak Mail (2397 NW Kings Blvd, Timberhill Shopping Ctr)</t>
-  </si>
-  <si>
-    <t>Parent Enhancement Program (421 NW 4th St)</t>
-  </si>
-  <si>
-    <t>Pastors for Peace-Caravan to Cuba (Mike Beilstein)</t>
-  </si>
-  <si>
-    <t>Philomath Community Garden (Chris Shonnard)</t>
-  </si>
-  <si>
-    <t>Philomath Community Srvcs (food &amp; kids stuff, 360 S 9th)</t>
-  </si>
-  <si>
-    <t>Play It Again Sports (1422 NW 9th St)</t>
-  </si>
-  <si>
-    <t>Presbyterian Piecemakers (cotton quilts)</t>
-  </si>
-  <si>
-    <t>Public Library Corvallis, Friends of (645 NW Monroe Ave) </t>
-  </si>
-  <si>
-    <t>Quilts From Caring Hands (cotton quilts)</t>
+    <t>Osborn Aquatic Center (1940 NW Highland Dr)44</t>
+  </si>
+  <si>
+    <t>OSU Emergency Food Pantry (2150 SW Jefferson Way)45</t>
+  </si>
+  <si>
+    <t>OSU Folk Club Thrift Shop (144 NW 2nd St)46</t>
+  </si>
+  <si>
+    <t>OSU Organic Growers Club (Crop &amp; Soil Science Dep't)47</t>
+  </si>
+  <si>
+    <t>Pak Mail (2397 NW Kings Blvd, Timberhill Shopping Ctr)48</t>
+  </si>
+  <si>
+    <t>Parent Enhancement Program (421 NW 4th St)49</t>
+  </si>
+  <si>
+    <t>Pastors for Peace-Caravan to Cuba (Mike Beilstein)50</t>
+  </si>
+  <si>
+    <t>Philomath Community Garden (Chris Shonnard)51</t>
+  </si>
+  <si>
+    <t>Philomath Community Srvcs (food &amp; kids stuff, 360 S 9th)52</t>
+  </si>
+  <si>
+    <t>Play It Again Sports (1422 NW 9th St)53</t>
+  </si>
+  <si>
+    <t>Presbyterian Piecemakers (cotton quilts)54</t>
+  </si>
+  <si>
+    <t>Public Library Corvallis, Friends of (645 NW Monroe Ave) 55</t>
+  </si>
+  <si>
+    <t>Quilts From Caring Hands (cotton quilts)56</t>
   </si>
   <si>
     <r>
@@ -445,11 +445,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(on NW 9th)</t>
+      <t xml:space="preserve">(on NW 9th)57</t>
     </r>
   </si>
   <si>
-    <t>Replay Children's Wear (260 NW 1st St)</t>
+    <t>Replay Children's Wear (260 NW 1st St)58</t>
   </si>
   <si>
     <r>
@@ -473,11 +473,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">volve (women's resale boutique, 103 SW 2nd St)</t>
+      <t xml:space="preserve">volve (women's resale boutique, 103 SW 2nd St)59</t>
     </r>
   </si>
   <si>
-    <t>Schools--Public, Private, Charter </t>
+    <t>Schools--Public, Private, Charter 60</t>
   </si>
   <si>
     <r>
@@ -491,14 +491,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> (SW 3rd &amp; SW Jefferson)</t>
+      <t xml:space="preserve"> (SW 3rd &amp; SW Jefferson)61</t>
     </r>
   </si>
   <si>
-    <t>Senior Center of Corvallis (2601 NW Tyler Ave)</t>
-  </si>
-  <si>
-    <t>South Corvallis Food Bank (1798 SW 3rd St)</t>
+    <t>Senior Center of Corvallis (2601 NW Tyler Ave)64</t>
+  </si>
+  <si>
+    <t>South Corvallis Food Bank (1798 SW 3rd St)65</t>
   </si>
   <si>
     <r>
@@ -512,11 +512,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(St Mary's Church, 25th St)</t>
+      <t xml:space="preserve">(St Mary's Church, 25th St)67</t>
     </r>
   </si>
   <si>
-    <t>UPS Stores (on NW Circle &amp; on SW Philomath Blvd) </t>
+    <t>UPS Stores (on NW Circle &amp; on SW Philomath Blvd) 68 69</t>
   </si>
   <si>
     <r>
@@ -538,11 +538,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(for low income citizens, 968 NW Garfield)</t>
+      <t xml:space="preserve">(for low income citizens, 968 NW Garfield)70</t>
     </r>
   </si>
   <si>
-    <t>Spaeth Heritage House (135 N 13th St, Philomath)</t>
+    <t>Spaeth Heritage House (135 N 13th St, Philomath)71</t>
   </si>
   <si>
     <t>ALWAYS CALL FIRST to confirm items are still being accepted!</t>
@@ -823,7 +823,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">BLDG MATERIALS / HOME IMPROVEMENT(CAT),(bID,6,)</t>
+      <t xml:space="preserve">BLDG MATERIALS / HOME IMPROVEMENT(CAT),(bID,6,45-67)</t>
     </r>
     <r>
       <rPr>
@@ -845,7 +845,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">CHILDREN'S GOODS / CLOTHING(bID,3,1)(bID,3,3)(bID,18-32)(bID,3,70) and</t>
+      <t xml:space="preserve">CHILDREN'S GOODS / CLOTHING(bID,3,1)(bID,3,3)(bID,3,18-32 except 30)(bID,3,70) and</t>
     </r>
     <r>
       <rPr>
@@ -1050,6 +1050,9 @@
     <t>Phone numbers </t>
   </si>
   <si>
+    <t>Albany-Corvallis ReUseIt (free items:  groups.yahoo.com)</t>
+  </si>
+  <si>
     <t>https://groups.yahoo.com/neo/groups/albanycorvallisReUseIt/info</t>
   </si>
   <si>
@@ -1116,6 +1119,9 @@
     <t>(888) 758-1121</t>
   </si>
   <si>
+    <t>Boys &amp; Girls Club / STARS (after school programs)</t>
+  </si>
+  <si>
     <t>1112 NW Circle Blvd</t>
   </si>
   <si>
@@ -1134,6 +1140,9 @@
     <t>541-760-5941</t>
   </si>
   <si>
+    <t>CARDV (Center Against Rape/Domestic Violence)</t>
+  </si>
+  <si>
     <t>4786 SW Philomath Blvd</t>
   </si>
   <si>
@@ -1185,6 +1194,9 @@
     <t>720 NE Granger Ave, Bldg J</t>
   </si>
   <si>
+    <t>Corvallis-Uzhhorod Sister Cities/The TOUCH Project</t>
+  </si>
+  <si>
     <t>http://www.sistercities.corvallis.or.us/uzhhorod</t>
   </si>
   <si>
@@ -1194,6 +1206,9 @@
     <t>138 SW 2nd St</t>
   </si>
   <si>
+    <t>Craigslist (corvallis.craigslist.org) and Freecycle.org</t>
+  </si>
+  <si>
     <t>https://corvallis.craigslist.org/</t>
   </si>
   <si>
@@ -1299,12 +1314,21 @@
     <t>2330 NW Professional Dr #102</t>
   </si>
   <si>
+    <t>Mario Pastega House (Good Sam patient family housing)</t>
+  </si>
+  <si>
     <t>3505 NW Samaritan Dr</t>
   </si>
   <si>
+    <t>Mary's River Gleaners (for low income citizens)</t>
+  </si>
+  <si>
     <t>Po Box 2309</t>
   </si>
   <si>
+    <t>Midway Farms (Hway 20 btw Corvallis &amp; Albany)</t>
+  </si>
+  <si>
     <t>6980 US-20</t>
   </si>
   <si>
@@ -1338,6 +1362,9 @@
     <t>541-752-4733</t>
   </si>
   <si>
+    <t>OSU Organic Growers Club (Crop &amp; Soil Science Dep't)</t>
+  </si>
+  <si>
     <t>http://cropandsoil.oregonstate.edu/organic_grower</t>
   </si>
   <si>
@@ -1353,9 +1380,15 @@
     <t>421 NW 4th St</t>
   </si>
   <si>
+    <t>Pastors for Peace-Caravan to Cuba (Mike Beilstein)</t>
+  </si>
+  <si>
     <t>www.ccds.org or www.ifconews.org.</t>
   </si>
   <si>
+    <t>Philomath Community Garden (Chris Shonnard)</t>
+  </si>
+  <si>
     <t>http://philomathcommunityservices.org/</t>
   </si>
   <si>
@@ -1371,6 +1404,9 @@
     <t>1422 NW 9th St</t>
   </si>
   <si>
+    <t>Presbyterian Piecemakers (cotton quilts)</t>
+  </si>
+  <si>
     <t>114 SW 8th St</t>
   </si>
   <si>
@@ -1380,6 +1416,9 @@
     <t>645 NW Monroe Ave</t>
   </si>
   <si>
+    <t>Quilts From Caring Hands (cotton quilts)</t>
+  </si>
+  <si>
     <t>1495 NW 20th St,</t>
   </si>
   <si>
@@ -1402,6 +1441,9 @@
   </si>
   <si>
     <t>103 SW 2nd St    </t>
+  </si>
+  <si>
+    <t>Schools--Public, Private, Charter </t>
   </si>
   <si>
     <t>Second Glance</t>
@@ -3532,13 +3574,13 @@
       <xdr:col>63</xdr:col>
       <xdr:colOff>58320</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>12960</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>117000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3553,7 +3595,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15779520" y="9592560"/>
+          <a:off x="15779520" y="10091880"/>
           <a:ext cx="145800" cy="151920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3571,13 +3613,13 @@
       <xdr:col>63</xdr:col>
       <xdr:colOff>58320</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>98280</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>12960</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3592,7 +3634,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15779520" y="9402120"/>
+          <a:off x="15779520" y="9901440"/>
           <a:ext cx="145800" cy="151920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3616,9 +3658,9 @@
   <dimension ref="1:39"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -9484,7 +9526,7 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
         <v>125</v>
       </c>
@@ -13712,7 +13754,7 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="42" t="s">
         <v>129</v>
       </c>
@@ -31612,7 +31654,7 @@
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="27" t="s">
         <v>148</v>
       </c>
@@ -40133,13 +40175,13 @@
     </row>
     <row r="2" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="62" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D2" s="64" t="s">
         <v>65</v>
@@ -40147,41 +40189,41 @@
     </row>
     <row r="3" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="62" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="62" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="62" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D5" s="64" t="s">
         <v>67</v>
@@ -40189,13 +40231,13 @@
     </row>
     <row r="6" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="62" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B6" s="62" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D6" s="64" t="s">
         <v>68</v>
@@ -40203,13 +40245,13 @@
     </row>
     <row r="7" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="62" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D7" s="64" t="s">
         <v>68</v>
@@ -40217,41 +40259,41 @@
     </row>
     <row r="8" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="62" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B8" s="66" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="62" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B9" s="66" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="62" t="s">
-        <v>7</v>
+        <v>186</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D10" s="64" t="s">
         <v>69</v>
@@ -40259,13 +40301,13 @@
     </row>
     <row r="11" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="62" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D11" s="64" t="s">
         <v>70</v>
@@ -40273,27 +40315,27 @@
     </row>
     <row r="12" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="62" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="62" t="s">
-        <v>9</v>
+        <v>193</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>71</v>
@@ -40301,13 +40343,13 @@
     </row>
     <row r="14" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="62" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D14" s="64" t="s">
         <v>72</v>
@@ -40315,13 +40357,13 @@
     </row>
     <row r="15" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="62" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D15" s="64" t="s">
         <v>73</v>
@@ -40329,13 +40371,13 @@
     </row>
     <row r="16" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="62" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D16" s="64" t="s">
         <v>74</v>
@@ -40343,13 +40385,13 @@
     </row>
     <row r="17" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="62" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D17" s="64" t="s">
         <v>75</v>
@@ -40357,13 +40399,13 @@
     </row>
     <row r="18" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="62" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D18" s="64" t="s">
         <v>76</v>
@@ -40371,13 +40413,13 @@
     </row>
     <row r="19" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="62" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D19" s="64" t="s">
         <v>77</v>
@@ -40385,13 +40427,13 @@
     </row>
     <row r="20" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="62" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D20" s="64" t="s">
         <v>78</v>
@@ -40399,13 +40441,13 @@
     </row>
     <row r="21" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="62" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D21" s="64" t="s">
         <v>79</v>
@@ -40413,13 +40455,13 @@
     </row>
     <row r="22" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="62" t="s">
-        <v>18</v>
+        <v>211</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D22" s="64" t="s">
         <v>80</v>
@@ -40427,13 +40469,13 @@
     </row>
     <row r="23" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="62" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D23" s="64" t="s">
         <v>81</v>
@@ -40441,13 +40483,13 @@
     </row>
     <row r="24" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="62" t="s">
-        <v>20</v>
+        <v>215</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D24" s="64" t="s">
         <v>65</v>
@@ -40455,13 +40497,13 @@
     </row>
     <row r="25" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="62" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D25" s="64" t="s">
         <v>82</v>
@@ -40469,13 +40511,13 @@
     </row>
     <row r="26" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="62" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B26" s="62" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D26" s="64" t="s">
         <v>82</v>
@@ -40483,27 +40525,27 @@
     </row>
     <row r="27" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="62" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="62" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B28" s="66" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D28" s="64" t="s">
         <v>83</v>
@@ -40511,13 +40553,13 @@
     </row>
     <row r="29" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="62" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D29" s="64" t="s">
         <v>84</v>
@@ -40525,41 +40567,41 @@
     </row>
     <row r="30" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="62" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B30" s="66" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C30" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="62" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B31" s="66" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D31" s="64" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="62" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D32" s="64" t="s">
         <v>85</v>
@@ -40567,13 +40609,13 @@
     </row>
     <row r="33" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="62" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B33" s="66" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D33" s="64" t="s">
         <v>86</v>
@@ -40581,13 +40623,13 @@
     </row>
     <row r="34" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="62" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B34" s="62" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D34" s="64" t="s">
         <v>87</v>
@@ -40595,13 +40637,13 @@
     </row>
     <row r="35" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="62" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B35" s="62" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D35" s="64" t="s">
         <v>88</v>
@@ -40609,13 +40651,13 @@
     </row>
     <row r="36" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="62" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B36" s="62" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C36" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D36" s="64" t="s">
         <v>89</v>
@@ -40623,13 +40665,13 @@
     </row>
     <row r="37" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="62" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B37" s="62" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D37" s="64" t="s">
         <v>90</v>
@@ -40637,13 +40679,13 @@
     </row>
     <row r="38" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="62" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B38" s="62" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D38" s="64" t="s">
         <v>91</v>
@@ -40651,13 +40693,13 @@
     </row>
     <row r="39" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="62" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B39" s="62" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C39" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D39" s="64" t="s">
         <v>92</v>
@@ -40665,13 +40707,13 @@
     </row>
     <row r="40" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="62" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B40" s="66" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D40" s="64" t="s">
         <v>93</v>
@@ -40679,13 +40721,13 @@
     </row>
     <row r="41" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="62" t="s">
-        <v>35</v>
+        <v>251</v>
       </c>
       <c r="B41" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C41" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D41" s="64" t="s">
         <v>94</v>
@@ -40694,13 +40736,13 @@
     </row>
     <row r="42" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="62" t="s">
-        <v>36</v>
+        <v>253</v>
       </c>
       <c r="B42" s="66" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="C42" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D42" s="68" t="s">
         <v>91</v>
@@ -40709,13 +40751,13 @@
     </row>
     <row r="43" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="62" t="s">
-        <v>37</v>
+        <v>255</v>
       </c>
       <c r="B43" s="62" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C43" s="63" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="D43" s="64" t="s">
         <v>95</v>
@@ -40724,13 +40766,13 @@
     </row>
     <row r="44" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="62" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B44" s="62" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C44" s="63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D44" s="64" t="s">
         <v>96</v>
@@ -40739,13 +40781,13 @@
     </row>
     <row r="45" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="62" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B45" s="62" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C45" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D45" s="64" t="s">
         <v>97</v>
@@ -40754,13 +40796,13 @@
     </row>
     <row r="46" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="62" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B46" s="62" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C46" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D46" s="64" t="s">
         <v>98</v>
@@ -40769,28 +40811,28 @@
     </row>
     <row r="47" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="62" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B47" s="62" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C47" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D47" s="64" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="E47" s="0"/>
     </row>
     <row r="48" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="62" t="s">
-        <v>42</v>
+        <v>267</v>
       </c>
       <c r="B48" s="69" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C48" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D48" s="64" t="s">
         <v>100</v>
@@ -40799,13 +40841,13 @@
     </row>
     <row r="49" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="62" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B49" s="62" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="C49" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D49" s="64" t="s">
         <v>101</v>
@@ -40815,13 +40857,13 @@
     </row>
     <row r="50" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="62" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="B50" s="62" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="C50" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D50" s="64" t="s">
         <v>102</v>
@@ -40831,13 +40873,13 @@
     </row>
     <row r="51" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="62" t="s">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="B51" s="62" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C51" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D51" s="64" t="s">
         <v>103</v>
@@ -40847,13 +40889,13 @@
     </row>
     <row r="52" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="62" t="s">
-        <v>46</v>
+        <v>275</v>
       </c>
       <c r="B52" s="62" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C52" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D52" s="64" t="s">
         <v>104</v>
@@ -40863,13 +40905,13 @@
     </row>
     <row r="53" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="62" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="B53" s="62" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="C53" s="63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D53" s="64" t="s">
         <v>105</v>
@@ -40879,13 +40921,13 @@
     </row>
     <row r="54" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="62" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="B54" s="62" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="C54" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D54" s="64" t="s">
         <v>106</v>
@@ -40895,13 +40937,13 @@
     </row>
     <row r="55" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="62" t="s">
-        <v>49</v>
+        <v>281</v>
       </c>
       <c r="B55" s="62" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="C55" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D55" s="64" t="s">
         <v>107</v>
@@ -40911,13 +40953,13 @@
     </row>
     <row r="56" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="62" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="B56" s="62" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="C56" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D56" s="64" t="s">
         <v>108</v>
@@ -40927,13 +40969,13 @@
     </row>
     <row r="57" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="62" t="s">
-        <v>51</v>
+        <v>285</v>
       </c>
       <c r="B57" s="66" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="C57" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D57" s="64" t="s">
         <v>109</v>
@@ -40943,29 +40985,29 @@
     </row>
     <row r="58" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="62" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B58" s="66" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="C58" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D58" s="64" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="E58" s="0"/>
       <c r="F58" s="59"/>
     </row>
     <row r="59" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="62" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="B59" s="62" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="C59" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D59" s="64" t="s">
         <v>110</v>
@@ -40975,13 +41017,13 @@
     </row>
     <row r="60" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="62" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="B60" s="62" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="C60" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D60" s="64" t="s">
         <v>111</v>
@@ -40991,13 +41033,13 @@
     </row>
     <row r="61" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="62" t="s">
-        <v>55</v>
+        <v>294</v>
       </c>
       <c r="B61" s="64" t="s">
         <v>66</v>
       </c>
       <c r="C61" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D61" s="64" t="s">
         <v>66</v>
@@ -41007,59 +41049,59 @@
     </row>
     <row r="62" s="65" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="62" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="B62" s="66" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="C62" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D62" s="64" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="E62" s="0"/>
       <c r="F62" s="59"/>
     </row>
     <row r="63" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="62" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="B63" s="64" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="C63" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D63" s="64" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="E63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="62" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="B64" s="62" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C64" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D64" s="64" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="E64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="62" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="B65" s="62" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="C65" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D65" s="64" t="s">
         <v>112</v>
@@ -41068,13 +41110,13 @@
     </row>
     <row r="66" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="62" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="B66" s="66" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="C66" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D66" s="64" t="s">
         <v>113</v>
@@ -41083,13 +41125,13 @@
     </row>
     <row r="67" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="73" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="B67" s="62" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="C67" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D67" s="64" t="s">
         <v>114</v>
@@ -41098,13 +41140,13 @@
     </row>
     <row r="68" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="62" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B68" s="73" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="C68" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D68" s="64" t="s">
         <v>114</v>
@@ -41112,43 +41154,43 @@
     </row>
     <row r="69" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="62" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="B69" s="62" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="C69" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D69" s="64" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="E69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="62" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="B70" s="62" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="C70" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D70" s="64" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="E70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="62" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="B71" s="62" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="C71" s="63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D71" s="64" t="s">
         <v>115</v>
@@ -41157,16 +41199,16 @@
     </row>
     <row r="72" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="62" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="B72" s="62" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="C72" s="63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D72" s="64" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -41188,8 +41230,8 @@
   </sheetPr>
   <dimension ref="1:25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42240,102 +42282,102 @@
     </row>
     <row r="2" s="77" customFormat="true" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="76" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
       <c r="C2" s="76" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="D2" s="76" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="E2" s="76" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="F2" s="76" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="G2" s="76" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="H2" s="76" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="I2" s="76" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="J2" s="76" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="K2" s="76" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="L2" s="76" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="M2" s="76" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="N2" s="76" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="O2" s="76" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
       <c r="P2" s="76" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" s="79" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="78" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="B3" s="78" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="C3" s="78" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="D3" s="78" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
       <c r="E3" s="78" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="F3" s="78" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="G3" s="78" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="I3" s="78" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="J3" s="78" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="K3" s="78" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="L3" s="78" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="M3" s="78" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="N3" s="78" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="O3" s="78" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="P3" s="78" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="Q3" s="79" t="n">
         <v>81</v>
@@ -42343,52 +42385,52 @@
     </row>
     <row r="4" s="79" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="78" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="B4" s="78" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="C4" s="78" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="D4" s="78" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="E4" s="78" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="F4" s="78" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="G4" s="78" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="H4" s="78" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
       <c r="I4" s="78" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="J4" s="78" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="K4" s="78" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="L4" s="78" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="M4" s="78" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="N4" s="78" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="O4" s="78" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="P4" s="78" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="Q4" s="79" t="n">
         <v>162</v>
@@ -42396,52 +42438,52 @@
     </row>
     <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="80" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="B5" s="78" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="C5" s="78" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="E5" s="78" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="F5" s="78" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="G5" s="78" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="H5" s="78" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="I5" s="78" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="J5" s="78" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="K5" s="78" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="L5" s="78" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="M5" s="78" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="N5" s="78" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="O5" s="78" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="P5" s="78" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="Q5" s="79" t="n">
         <v>3</v>
@@ -42449,96 +42491,96 @@
     </row>
     <row r="6" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="80" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="C6" s="78" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="D6" s="78" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="E6" s="78" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="F6" s="78" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="G6" s="78" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="H6" s="78" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="I6" s="78" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="J6" s="78" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="K6" s="78" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="L6" s="78" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="M6" s="78" t="s">
-        <v>382</v>
+        <v>396</v>
       </c>
       <c r="N6" s="78"/>
       <c r="O6" s="78" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="P6" s="78" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="80" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C7" s="78" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="D7" s="78" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="E7" s="78" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="F7" s="78" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="G7" s="78" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="H7" s="78" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="I7" s="78" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="J7" s="78" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="K7" s="78"/>
       <c r="L7" s="78" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="M7" s="78" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="N7" s="78"/>
       <c r="O7" s="81" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="P7" s="78" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="Q7" s="79" t="n">
         <v>70</v>
@@ -42546,46 +42588,46 @@
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="80" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="B8" s="78" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="C8" s="78" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="D8" s="78" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="E8" s="78"/>
       <c r="F8" s="78" t="s">
-        <v>402</v>
+        <v>416</v>
       </c>
       <c r="G8" s="78" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="H8" s="78" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="I8" s="78" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="J8" s="78" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="K8" s="78"/>
       <c r="L8" s="78" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="M8" s="78" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="N8" s="78"/>
       <c r="O8" s="78" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="P8" s="78" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="Q8" s="79" t="n">
         <v>82</v>
@@ -42593,44 +42635,44 @@
     </row>
     <row r="9" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="78" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="B9" s="82"/>
       <c r="C9" s="78" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="D9" s="78" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
       <c r="E9" s="78"/>
       <c r="F9" s="78" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="G9" s="78" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
       <c r="H9" s="78" t="s">
-        <v>415</v>
+        <v>429</v>
       </c>
       <c r="I9" s="78" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="J9" s="78" t="s">
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="K9" s="78"/>
       <c r="L9" s="78" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="M9" s="78" t="s">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="N9" s="78"/>
       <c r="O9" s="78" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="P9" s="78" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="Q9" s="79" t="n">
         <v>11</v>
@@ -42638,42 +42680,42 @@
     </row>
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="80" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="B10" s="82"/>
       <c r="C10" s="78" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="D10" s="83"/>
       <c r="E10" s="78"/>
       <c r="F10" s="78" t="s">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="G10" s="78" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
       <c r="H10" s="78" t="s">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="I10" s="78" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="J10" s="78" t="s">
-        <v>427</v>
+        <v>441</v>
       </c>
       <c r="K10" s="78"/>
       <c r="L10" s="78" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="M10" s="80" t="s">
-        <v>429</v>
+        <v>443</v>
       </c>
       <c r="N10" s="78"/>
       <c r="O10" s="78" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="P10" s="78" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="Q10" s="79" t="n">
         <v>163</v>
@@ -42681,40 +42723,40 @@
     </row>
     <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="80" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="B11" s="82"/>
       <c r="C11" s="78" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="D11" s="83"/>
       <c r="E11" s="78"/>
       <c r="F11" s="78" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="G11" s="82"/>
       <c r="H11" s="78" t="s">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="I11" s="78" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="J11" s="78" t="s">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="K11" s="78"/>
       <c r="L11" s="78" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="M11" s="78" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="N11" s="78"/>
       <c r="O11" s="78" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="P11" s="78" t="s">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="Q11" s="79" t="n">
         <v>164</v>
@@ -42722,38 +42764,38 @@
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="80" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="B12" s="82"/>
       <c r="C12" s="78" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="D12" s="83"/>
       <c r="E12" s="78"/>
       <c r="F12" s="78" t="s">
-        <v>443</v>
+        <v>457</v>
       </c>
       <c r="G12" s="82"/>
       <c r="H12" s="78" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="I12" s="78" t="s">
-        <v>445</v>
+        <v>459</v>
       </c>
       <c r="J12" s="78" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="K12" s="78"/>
       <c r="L12" s="78" t="s">
-        <v>447</v>
+        <v>461</v>
       </c>
       <c r="M12" s="78" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="N12" s="78"/>
       <c r="O12" s="78"/>
       <c r="P12" s="78" t="s">
-        <v>449</v>
+        <v>463</v>
       </c>
       <c r="Q12" s="79" t="n">
         <v>165</v>
@@ -42761,40 +42803,40 @@
     </row>
     <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="80" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="B13" s="82"/>
       <c r="C13" s="78" t="s">
-        <v>451</v>
+        <v>465</v>
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="78"/>
       <c r="F13" s="78" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="G13" s="82"/>
       <c r="H13" s="78" t="s">
-        <v>453</v>
+        <v>467</v>
       </c>
       <c r="I13" s="78" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="J13" s="78" t="s">
-        <v>455</v>
+        <v>469</v>
       </c>
       <c r="K13" s="78"/>
       <c r="L13" s="78" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="M13" s="78" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="N13" s="78"/>
       <c r="O13" s="78" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="P13" s="78" t="s">
-        <v>459</v>
+        <v>473</v>
       </c>
       <c r="Q13" s="79" t="n">
         <v>74</v>
@@ -42802,38 +42844,38 @@
     </row>
     <row r="14" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="80" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="B14" s="82"/>
       <c r="C14" s="78" t="s">
-        <v>461</v>
+        <v>475</v>
       </c>
       <c r="D14" s="83"/>
       <c r="E14" s="78"/>
       <c r="F14" s="78" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="G14" s="82"/>
       <c r="H14" s="78" t="s">
-        <v>463</v>
+        <v>477</v>
       </c>
       <c r="I14" s="78" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="J14" s="78" t="s">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="K14" s="78"/>
       <c r="L14" s="78" t="s">
-        <v>466</v>
+        <v>480</v>
       </c>
       <c r="M14" s="78"/>
       <c r="N14" s="78"/>
       <c r="O14" s="78" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="P14" s="78" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="Q14" s="79" t="n">
         <v>75</v>
@@ -42844,26 +42886,26 @@
     </row>
     <row r="15" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="80" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="B15" s="82"/>
       <c r="C15" s="78" t="s">
-        <v>470</v>
+        <v>484</v>
       </c>
       <c r="D15" s="83"/>
       <c r="E15" s="78"/>
       <c r="F15" s="78" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="G15" s="82"/>
       <c r="H15" s="78" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="I15" s="78" t="s">
-        <v>472</v>
+        <v>486</v>
       </c>
       <c r="J15" s="78" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="K15" s="78"/>
       <c r="L15" s="78"/>
@@ -42871,7 +42913,7 @@
       <c r="N15" s="78"/>
       <c r="O15" s="78"/>
       <c r="P15" s="78" t="s">
-        <v>474</v>
+        <v>488</v>
       </c>
       <c r="Q15" s="79" t="n">
         <v>166</v>
@@ -42879,26 +42921,26 @@
     </row>
     <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="80" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="B16" s="82"/>
       <c r="C16" s="78" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="D16" s="83"/>
       <c r="E16" s="78"/>
       <c r="F16" s="78" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="G16" s="82"/>
       <c r="H16" s="78" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="I16" s="78" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="J16" s="78" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
       <c r="K16" s="78"/>
       <c r="L16" s="78"/>
@@ -42906,7 +42948,7 @@
       <c r="N16" s="78"/>
       <c r="O16" s="78"/>
       <c r="P16" s="78" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="Q16" s="79" t="n">
         <v>167</v>
@@ -42914,23 +42956,23 @@
     </row>
     <row r="17" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="80" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="B17" s="82"/>
       <c r="C17" s="78" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="D17" s="83"/>
       <c r="E17" s="78"/>
       <c r="F17" s="78" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="G17" s="82"/>
       <c r="H17" s="78" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="I17" s="78" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="J17" s="78"/>
       <c r="K17" s="78"/>
@@ -42942,23 +42984,23 @@
     </row>
     <row r="18" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="80" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="B18" s="82"/>
       <c r="C18" s="78" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="D18" s="83"/>
       <c r="E18" s="78"/>
       <c r="F18" s="78" t="s">
-        <v>488</v>
+        <v>502</v>
       </c>
       <c r="G18" s="82"/>
       <c r="H18" s="78" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="I18" s="78" t="s">
-        <v>490</v>
+        <v>504</v>
       </c>
       <c r="J18" s="78"/>
       <c r="K18" s="78"/>
@@ -42970,23 +43012,23 @@
     </row>
     <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="80" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="B19" s="82"/>
       <c r="C19" s="78" t="s">
-        <v>492</v>
+        <v>506</v>
       </c>
       <c r="D19" s="83"/>
       <c r="E19" s="78"/>
       <c r="F19" s="78" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="G19" s="82"/>
       <c r="H19" s="78" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="I19" s="78" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="J19" s="78"/>
       <c r="K19" s="78"/>
@@ -43000,19 +43042,19 @@
       <c r="A20" s="80"/>
       <c r="B20" s="82"/>
       <c r="C20" s="78" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
       <c r="D20" s="83"/>
       <c r="E20" s="78"/>
       <c r="F20" s="78" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="G20" s="82"/>
       <c r="H20" s="78" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="I20" s="78" t="s">
-        <v>498</v>
+        <v>512</v>
       </c>
       <c r="J20" s="78"/>
       <c r="K20" s="78"/>
@@ -43029,14 +43071,14 @@
       <c r="D21" s="83"/>
       <c r="E21" s="78"/>
       <c r="F21" s="78" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="G21" s="82"/>
       <c r="H21" s="78" t="s">
-        <v>500</v>
+        <v>514</v>
       </c>
       <c r="I21" s="78" t="s">
-        <v>501</v>
+        <v>515</v>
       </c>
       <c r="J21" s="78"/>
       <c r="K21" s="78"/>
@@ -43053,11 +43095,11 @@
       <c r="D22" s="83"/>
       <c r="E22" s="78"/>
       <c r="F22" s="78" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="G22" s="82"/>
       <c r="H22" s="78" t="s">
-        <v>502</v>
+        <v>516</v>
       </c>
       <c r="I22" s="78"/>
       <c r="J22" s="78"/>
@@ -43075,11 +43117,11 @@
       <c r="D23" s="83"/>
       <c r="E23" s="78"/>
       <c r="F23" s="78" t="s">
-        <v>503</v>
+        <v>517</v>
       </c>
       <c r="G23" s="82"/>
       <c r="H23" s="78" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="I23" s="78"/>
       <c r="J23" s="78"/>
@@ -43097,11 +43139,11 @@
       <c r="D24" s="83"/>
       <c r="E24" s="78"/>
       <c r="F24" s="78" t="s">
-        <v>504</v>
+        <v>518</v>
       </c>
       <c r="G24" s="82"/>
       <c r="H24" s="78" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="I24" s="78"/>
       <c r="J24" s="78"/>
@@ -43119,7 +43161,7 @@
       <c r="D25" s="83"/>
       <c r="E25" s="78"/>
       <c r="F25" s="78" t="s">
-        <v>506</v>
+        <v>520</v>
       </c>
       <c r="G25" s="82"/>
       <c r="H25" s="78"/>
@@ -43168,25 +43210,25 @@
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="87" t="s">
-        <v>507</v>
+        <v>521</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>508</v>
+        <v>522</v>
       </c>
       <c r="C1" s="87" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="D1" s="87" t="s">
-        <v>510</v>
+        <v>524</v>
       </c>
       <c r="E1" s="87" t="s">
-        <v>511</v>
+        <v>525</v>
       </c>
       <c r="F1" s="87" t="s">
-        <v>512</v>
+        <v>526</v>
       </c>
       <c r="G1" s="87" t="s">
-        <v>513</v>
+        <v>527</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43194,22 +43236,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="90" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="C2" s="91" t="s">
-        <v>514</v>
+        <v>528</v>
       </c>
       <c r="D2" s="91" t="s">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>516</v>
+        <v>530</v>
       </c>
       <c r="F2" s="91" t="s">
-        <v>517</v>
+        <v>531</v>
       </c>
       <c r="G2" s="91" t="s">
-        <v>518</v>
+        <v>532</v>
       </c>
       <c r="H2" s="0"/>
     </row>
@@ -43218,22 +43260,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="90" t="s">
-        <v>519</v>
+        <v>533</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>520</v>
+        <v>534</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>521</v>
+        <v>535</v>
       </c>
       <c r="E3" s="91" t="s">
-        <v>522</v>
+        <v>536</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>523</v>
+        <v>537</v>
       </c>
       <c r="G3" s="91" t="s">
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="H3" s="0"/>
     </row>
@@ -43242,22 +43284,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>519</v>
+        <v>533</v>
       </c>
       <c r="C4" s="91" t="s">
-        <v>525</v>
+        <v>539</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>526</v>
+        <v>540</v>
       </c>
       <c r="E4" s="91" t="s">
-        <v>527</v>
+        <v>541</v>
       </c>
       <c r="F4" s="93" t="s">
-        <v>528</v>
+        <v>542</v>
       </c>
       <c r="G4" s="91" t="s">
-        <v>529</v>
+        <v>543</v>
       </c>
       <c r="H4" s="94" t="s">
         <v>121</v>
@@ -43268,22 +43310,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="90" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="C5" s="91" t="s">
-        <v>530</v>
+        <v>544</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>531</v>
+        <v>545</v>
       </c>
       <c r="E5" s="91" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="F5" s="91" t="s">
-        <v>533</v>
+        <v>547</v>
       </c>
       <c r="G5" s="91" t="s">
-        <v>534</v>
+        <v>548</v>
       </c>
       <c r="H5" s="94"/>
     </row>
@@ -43292,22 +43334,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="95" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="C6" s="91" t="s">
-        <v>535</v>
+        <v>549</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>536</v>
+        <v>550</v>
       </c>
       <c r="E6" s="91" t="s">
-        <v>537</v>
+        <v>551</v>
       </c>
       <c r="F6" s="91" t="s">
-        <v>538</v>
+        <v>552</v>
       </c>
       <c r="G6" s="91" t="s">
-        <v>539</v>
+        <v>553</v>
       </c>
       <c r="H6" s="94"/>
     </row>
@@ -43316,22 +43358,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="95" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>540</v>
+        <v>554</v>
       </c>
       <c r="D7" s="91" t="s">
-        <v>541</v>
+        <v>555</v>
       </c>
       <c r="E7" s="91" t="s">
-        <v>542</v>
+        <v>556</v>
       </c>
       <c r="F7" s="91" t="s">
-        <v>543</v>
+        <v>557</v>
       </c>
       <c r="G7" s="91" t="s">
-        <v>544</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43339,22 +43381,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>545</v>
+        <v>559</v>
       </c>
       <c r="C8" s="91" t="s">
-        <v>525</v>
+        <v>539</v>
       </c>
       <c r="D8" s="91" t="s">
-        <v>526</v>
+        <v>540</v>
       </c>
       <c r="E8" s="91" t="s">
-        <v>527</v>
+        <v>541</v>
       </c>
       <c r="F8" s="93" t="s">
-        <v>528</v>
+        <v>542</v>
       </c>
       <c r="G8" s="91" t="s">
-        <v>529</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43362,22 +43404,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>546</v>
+        <v>560</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>547</v>
+        <v>561</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="E9" s="97" t="s">
-        <v>549</v>
+        <v>563</v>
       </c>
       <c r="F9" s="91" t="s">
-        <v>550</v>
+        <v>564</v>
       </c>
       <c r="G9" s="98" t="s">
-        <v>551</v>
+        <v>565</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43385,22 +43427,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="95" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>552</v>
+        <v>566</v>
       </c>
       <c r="D10" s="91" t="s">
-        <v>553</v>
+        <v>567</v>
       </c>
       <c r="E10" s="99" t="s">
-        <v>554</v>
+        <v>568</v>
       </c>
       <c r="F10" s="91" t="s">
-        <v>555</v>
+        <v>569</v>
       </c>
       <c r="G10" s="91" t="s">
-        <v>556</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43408,22 +43450,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="95" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="C11" s="91" t="s">
-        <v>557</v>
+        <v>571</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>558</v>
+        <v>572</v>
       </c>
       <c r="E11" s="91" t="s">
-        <v>559</v>
+        <v>573</v>
       </c>
       <c r="F11" s="91" t="s">
-        <v>560</v>
+        <v>574</v>
       </c>
       <c r="G11" s="91" t="s">
-        <v>561</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43431,22 +43473,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>562</v>
+        <v>576</v>
       </c>
       <c r="C12" s="91" t="s">
-        <v>563</v>
+        <v>577</v>
       </c>
       <c r="D12" s="91" t="s">
-        <v>564</v>
+        <v>578</v>
       </c>
       <c r="E12" s="91" t="s">
-        <v>565</v>
+        <v>579</v>
       </c>
       <c r="F12" s="91" t="s">
-        <v>566</v>
+        <v>580</v>
       </c>
       <c r="G12" s="91" t="s">
-        <v>567</v>
+        <v>581</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43454,22 +43496,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>568</v>
+        <v>582</v>
       </c>
       <c r="C13" s="91" t="s">
-        <v>569</v>
+        <v>583</v>
       </c>
       <c r="D13" s="100" t="s">
-        <v>570</v>
+        <v>584</v>
       </c>
       <c r="E13" s="91" t="s">
-        <v>571</v>
+        <v>585</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>572</v>
+        <v>586</v>
       </c>
       <c r="G13" s="91" t="s">
-        <v>573</v>
+        <v>587</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43477,22 +43519,22 @@
         <v>14</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>574</v>
+        <v>588</v>
       </c>
       <c r="C14" s="91" t="s">
-        <v>575</v>
+        <v>589</v>
       </c>
       <c r="D14" s="91" t="s">
-        <v>576</v>
+        <v>590</v>
       </c>
       <c r="E14" s="91" t="s">
-        <v>577</v>
+        <v>591</v>
       </c>
       <c r="F14" s="101" t="s">
-        <v>578</v>
+        <v>592</v>
       </c>
       <c r="G14" s="91" t="s">
-        <v>579</v>
+        <v>593</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43500,22 +43542,22 @@
         <v>15</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>580</v>
+        <v>594</v>
       </c>
       <c r="C15" s="91" t="s">
-        <v>569</v>
+        <v>583</v>
       </c>
       <c r="D15" s="100" t="s">
-        <v>570</v>
+        <v>584</v>
       </c>
       <c r="E15" s="91" t="s">
-        <v>571</v>
+        <v>585</v>
       </c>
       <c r="F15" s="91" t="s">
-        <v>572</v>
+        <v>586</v>
       </c>
       <c r="G15" s="91" t="s">
-        <v>581</v>
+        <v>595</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43523,22 +43565,22 @@
         <v>16</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="C16" s="91" t="s">
-        <v>582</v>
+        <v>596</v>
       </c>
       <c r="D16" s="91" t="s">
-        <v>583</v>
+        <v>597</v>
       </c>
       <c r="E16" s="91" t="s">
-        <v>584</v>
+        <v>598</v>
       </c>
       <c r="F16" s="91" t="s">
-        <v>585</v>
+        <v>599</v>
       </c>
       <c r="G16" s="91" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43546,22 +43588,22 @@
         <v>18</v>
       </c>
       <c r="B17" s="95" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="C17" s="91" t="s">
-        <v>587</v>
+        <v>601</v>
       </c>
       <c r="D17" s="91" t="s">
-        <v>588</v>
+        <v>602</v>
       </c>
       <c r="E17" s="91" t="s">
-        <v>589</v>
+        <v>603</v>
       </c>
       <c r="F17" s="91" t="s">
-        <v>590</v>
+        <v>604</v>
       </c>
       <c r="G17" s="91" t="s">
-        <v>591</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>